<commit_message>
Added Loading Component to all the App
</commit_message>
<xml_diff>
--- a/com.Goval.FacturaDigital/com.Goval.FacturaDigital.Android/Reports/FacturaGoval.xlsx
+++ b/com.Goval.FacturaDigital/com.Goval.FacturaDigital.Android/Reports/FacturaGoval.xlsx
@@ -769,6 +769,45 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="3" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -780,15 +819,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -831,36 +861,6 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1234,8 +1234,8 @@
   </sheetPr>
   <dimension ref="A1:T441"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="13.2"/>
@@ -1298,16 +1298,16 @@
         <v>17</v>
       </c>
       <c r="J3" s="4"/>
-      <c r="K3" s="86"/>
-      <c r="L3" s="86"/>
-      <c r="M3" s="86"/>
-      <c r="N3" s="86"/>
-      <c r="O3" s="86"/>
-      <c r="P3" s="86"/>
-      <c r="Q3" s="86"/>
-      <c r="R3" s="86"/>
-      <c r="S3" s="86"/>
-      <c r="T3" s="86"/>
+      <c r="K3" s="99"/>
+      <c r="L3" s="99"/>
+      <c r="M3" s="99"/>
+      <c r="N3" s="99"/>
+      <c r="O3" s="99"/>
+      <c r="P3" s="99"/>
+      <c r="Q3" s="99"/>
+      <c r="R3" s="99"/>
+      <c r="S3" s="99"/>
+      <c r="T3" s="99"/>
     </row>
     <row r="4" spans="1:20" ht="20.100000000000001" customHeight="1">
       <c r="A4" s="31" t="s">
@@ -1439,17 +1439,17 @@
       <c r="K11" s="1"/>
     </row>
     <row r="12" spans="1:20" ht="15" customHeight="1">
-      <c r="A12" s="98" t="s">
+      <c r="A12" s="108" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="100"/>
+      <c r="B12" s="110"/>
       <c r="C12" s="70"/>
-      <c r="D12" s="98" t="s">
+      <c r="D12" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="99"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="100"/>
+      <c r="E12" s="109"/>
+      <c r="F12" s="109"/>
+      <c r="G12" s="110"/>
       <c r="H12" s="34" t="s">
         <v>10</v>
       </c>
@@ -1462,15 +1462,15 @@
       <c r="K12" s="1"/>
     </row>
     <row r="13" spans="1:20" ht="15" customHeight="1">
-      <c r="A13" s="96"/>
-      <c r="B13" s="97"/>
+      <c r="A13" s="106"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="71"/>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="106" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="101"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="97"/>
+      <c r="E13" s="111"/>
+      <c r="F13" s="111"/>
+      <c r="G13" s="107"/>
       <c r="H13" s="32" t="s">
         <v>11</v>
       </c>
@@ -1482,21 +1482,21 @@
       <c r="M13" s="81"/>
     </row>
     <row r="14" spans="1:20" ht="15" customHeight="1">
-      <c r="A14" s="83"/>
-      <c r="B14" s="84"/>
+      <c r="A14" s="96"/>
+      <c r="B14" s="97"/>
       <c r="C14" s="15"/>
-      <c r="D14" s="111"/>
-      <c r="E14" s="112"/>
-      <c r="F14" s="112"/>
-      <c r="G14" s="113"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="87"/>
       <c r="H14" s="16"/>
       <c r="I14" s="33"/>
       <c r="J14" s="78"/>
       <c r="K14" s="1"/>
     </row>
     <row r="15" spans="1:20" ht="15" customHeight="1">
-      <c r="A15" s="109"/>
-      <c r="B15" s="110"/>
+      <c r="A15" s="83"/>
+      <c r="B15" s="84"/>
       <c r="C15" s="39"/>
       <c r="D15" s="27"/>
       <c r="E15" s="30"/>
@@ -1585,8 +1585,8 @@
       <c r="O20" s="18"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1">
-      <c r="A21" s="109"/>
-      <c r="B21" s="110"/>
+      <c r="A21" s="83"/>
+      <c r="B21" s="84"/>
       <c r="C21" s="39"/>
       <c r="D21" s="27"/>
       <c r="E21" s="30"/>
@@ -1600,8 +1600,8 @@
       <c r="O21" s="17"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1">
-      <c r="A22" s="109"/>
-      <c r="B22" s="110"/>
+      <c r="A22" s="83"/>
+      <c r="B22" s="84"/>
       <c r="C22" s="39"/>
       <c r="D22" s="27"/>
       <c r="E22" s="30"/>
@@ -1630,8 +1630,8 @@
       <c r="O23" s="18"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1">
-      <c r="A24" s="109"/>
-      <c r="B24" s="110"/>
+      <c r="A24" s="83"/>
+      <c r="B24" s="84"/>
       <c r="C24" s="39"/>
       <c r="D24" s="27"/>
       <c r="E24" s="30"/>
@@ -1645,8 +1645,8 @@
       <c r="O24" s="18"/>
     </row>
     <row r="25" spans="1:15" ht="15" customHeight="1">
-      <c r="A25" s="109"/>
-      <c r="B25" s="110"/>
+      <c r="A25" s="83"/>
+      <c r="B25" s="84"/>
       <c r="C25" s="39"/>
       <c r="D25" s="27"/>
       <c r="E25" s="30"/>
@@ -1660,8 +1660,8 @@
       <c r="O25" s="17"/>
     </row>
     <row r="26" spans="1:15" ht="15" customHeight="1">
-      <c r="A26" s="109"/>
-      <c r="B26" s="110"/>
+      <c r="A26" s="83"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="39"/>
       <c r="D26" s="27"/>
       <c r="E26" s="30"/>
@@ -1705,41 +1705,41 @@
       <c r="O28" s="18"/>
     </row>
     <row r="29" spans="1:15" ht="15" customHeight="1">
-      <c r="A29" s="107"/>
-      <c r="B29" s="108"/>
+      <c r="A29" s="94"/>
+      <c r="B29" s="95"/>
       <c r="C29" s="39"/>
-      <c r="D29" s="87" t="s">
+      <c r="D29" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="E29" s="88"/>
-      <c r="F29" s="88"/>
-      <c r="G29" s="89"/>
+      <c r="E29" s="92"/>
+      <c r="F29" s="92"/>
+      <c r="G29" s="93"/>
       <c r="H29" s="73"/>
       <c r="I29" s="33"/>
       <c r="J29" s="79"/>
       <c r="K29" s="1"/>
     </row>
     <row r="30" spans="1:15" ht="15" customHeight="1">
-      <c r="A30" s="107"/>
-      <c r="B30" s="108"/>
+      <c r="A30" s="94"/>
+      <c r="B30" s="95"/>
       <c r="C30" s="39"/>
-      <c r="D30" s="87"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="89"/>
+      <c r="D30" s="91"/>
+      <c r="E30" s="92"/>
+      <c r="F30" s="92"/>
+      <c r="G30" s="93"/>
       <c r="H30" s="73"/>
       <c r="I30" s="33"/>
       <c r="J30" s="79"/>
       <c r="K30" s="1"/>
     </row>
     <row r="31" spans="1:15" ht="15" customHeight="1">
-      <c r="A31" s="102"/>
-      <c r="B31" s="103"/>
+      <c r="A31" s="112"/>
+      <c r="B31" s="113"/>
       <c r="C31" s="74"/>
-      <c r="D31" s="104"/>
-      <c r="E31" s="105"/>
-      <c r="F31" s="105"/>
-      <c r="G31" s="106"/>
+      <c r="D31" s="88"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="89"/>
+      <c r="G31" s="90"/>
       <c r="H31" s="75"/>
       <c r="I31" s="42"/>
       <c r="J31" s="80"/>
@@ -1766,10 +1766,10 @@
       <c r="E33" s="43"/>
       <c r="F33" s="43"/>
       <c r="G33" s="43"/>
-      <c r="H33" s="90" t="s">
+      <c r="H33" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="91"/>
+      <c r="I33" s="101"/>
       <c r="J33" s="51"/>
       <c r="K33" s="1"/>
       <c r="N33" s="21"/>
@@ -1783,10 +1783,10 @@
       <c r="E34" s="43"/>
       <c r="F34" s="43"/>
       <c r="G34" s="43"/>
-      <c r="H34" s="94" t="s">
+      <c r="H34" s="104" t="s">
         <v>6</v>
       </c>
-      <c r="I34" s="95"/>
+      <c r="I34" s="105"/>
       <c r="J34" s="52"/>
       <c r="K34" s="1"/>
       <c r="N34" s="21"/>
@@ -1802,10 +1802,10 @@
       <c r="E35" s="54"/>
       <c r="F35" s="54"/>
       <c r="G35" s="43"/>
-      <c r="H35" s="94" t="s">
+      <c r="H35" s="104" t="s">
         <v>3</v>
       </c>
-      <c r="I35" s="95"/>
+      <c r="I35" s="105"/>
       <c r="J35" s="52"/>
       <c r="K35" s="1"/>
       <c r="N35" s="21"/>
@@ -1818,11 +1818,11 @@
       <c r="D36" s="55"/>
       <c r="E36" s="55"/>
       <c r="F36" s="55"/>
-      <c r="G36" s="43"/>
-      <c r="H36" s="94" t="s">
+      <c r="G36" s="55"/>
+      <c r="H36" s="104" t="s">
         <v>5</v>
       </c>
-      <c r="I36" s="95"/>
+      <c r="I36" s="105"/>
       <c r="J36" s="52"/>
       <c r="K36" s="1"/>
       <c r="N36" s="21"/>
@@ -1836,10 +1836,10 @@
       <c r="E37" s="54"/>
       <c r="F37" s="54"/>
       <c r="G37" s="43"/>
-      <c r="H37" s="92" t="s">
+      <c r="H37" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="I37" s="93"/>
+      <c r="I37" s="103"/>
       <c r="J37" s="53"/>
       <c r="K37" s="1"/>
       <c r="N37" s="21"/>
@@ -1981,10 +1981,10 @@
       </c>
       <c r="B46" s="60"/>
       <c r="C46" s="60"/>
-      <c r="D46" s="85" t="s">
+      <c r="D46" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="E46" s="85"/>
+      <c r="E46" s="98"/>
       <c r="F46" s="61" t="s">
         <v>37</v>
       </c>
@@ -2002,10 +2002,10 @@
       </c>
       <c r="B47" s="60"/>
       <c r="C47" s="60"/>
-      <c r="D47" s="85" t="s">
+      <c r="D47" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="E47" s="85"/>
+      <c r="E47" s="98"/>
       <c r="F47" s="61" t="s">
         <v>37</v>
       </c>
@@ -2023,10 +2023,10 @@
       </c>
       <c r="B48" s="60"/>
       <c r="C48" s="60"/>
-      <c r="D48" s="85" t="s">
+      <c r="D48" s="98" t="s">
         <v>36</v>
       </c>
-      <c r="E48" s="85"/>
+      <c r="E48" s="98"/>
       <c r="F48" s="61" t="s">
         <v>37</v>
       </c>
@@ -8316,18 +8316,11 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D14:G14"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D30:G30"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="D13:G13"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
@@ -8338,11 +8331,18 @@
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H35:I35"/>
     <mergeCell ref="H34:I34"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="D13:G13"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D30:G30"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D14:G14"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>